<commit_message>
Import to dbIdc excel files
</commit_message>
<xml_diff>
--- a/ProLeiTAG/Massafra/Update/Values/Procedures/Decoction Line A - 99RP/Sequence 03 - Malt Outtake/99RP264_S03_Handler.xlsx
+++ b/ProLeiTAG/Massafra/Update/Values/Procedures/Decoction Line A - 99RP/Sequence 03 - Malt Outtake/99RP264_S03_Handler.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dso/ProLeiT/Massafra/MassafraSQL/ProLeiTAG/Massafra/Update/Values/Procedures/Decoction Line A - 99RP/Sequence 03 - Malt Outtake/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3541B24A-CD61-7648-8E51-1737914D3751}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05801DB6-A1A9-044A-BCF6-1EE481002767}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9520" yWindow="-21140" windowWidth="51200" windowHeight="21140" activeTab="6" xr2:uid="{D1D26D2E-F865-E045-8F90-C0A773A3A1DA}"/>
+    <workbookView xWindow="-9520" yWindow="-21600" windowWidth="51200" windowHeight="21600" firstSheet="1" activeTab="4" xr2:uid="{D1D26D2E-F865-E045-8F90-C0A773A3A1DA}"/>
   </bookViews>
   <sheets>
     <sheet name="00 Value Source" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1960" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1933" uniqueCount="276">
   <si>
     <r>
       <t xml:space="preserve">UPDATE </t>
@@ -992,6 +992,30 @@
   <si>
     <t>SET ExportClearance   = 2</t>
   </si>
+  <si>
+    <t>26: Milling Time</t>
+  </si>
+  <si>
+    <t>25: Initial Malt to Maize Amount</t>
+  </si>
+  <si>
+    <t>025: Silo Nr  Outtake 1</t>
+  </si>
+  <si>
+    <t>027: Silo Nr Outtake 2</t>
+  </si>
+  <si>
+    <t>029: Silo Nr Outtake 3</t>
+  </si>
+  <si>
+    <t>031: Silo Nr Outtake 4</t>
+  </si>
+  <si>
+    <t>033: Silo Nr Outtake Special</t>
+  </si>
+  <si>
+    <t>035: Silo Nr Outtake Colorato</t>
+  </si>
 </sst>
 </file>
 
@@ -1062,7 +1086,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1114,6 +1138,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1277,7 +1313,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1382,6 +1418,10 @@
     <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7507,21 +7547,21 @@
     <row r="2" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="38" t="str">
         <f>CONCATENATE(B2,C2,D2,E2)</f>
-        <v xml:space="preserve">-- Function: Massafra -   | Bergamo - </v>
+        <v>-- Function: Massafra -  SeqRunTime | Bergamo - 01: SeqRunTime</v>
       </c>
       <c r="B2" s="21" t="s">
         <v>31</v>
       </c>
       <c r="C2" s="29" t="str">
         <f>IF('01 Function Comparison'!$K$3="NULL","",IF(ISBLANK('01 Function Comparison'!$K$3),"",'01 Function Comparison'!$K$3))</f>
-        <v/>
+        <v>SeqRunTime</v>
       </c>
       <c r="D2" s="25" t="s">
         <v>23</v>
       </c>
       <c r="E2" s="34" t="str">
         <f>IF(ISBLANK('01 Function Comparison'!$G$3),"",'01 Function Comparison'!$G$3)</f>
-        <v/>
+        <v>01: SeqRunTime</v>
       </c>
       <c r="F2" s="42"/>
     </row>
@@ -7548,23 +7588,23 @@
     <row r="5" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="40" t="str">
         <f>CONCATENATE(D5,E5)</f>
-        <v xml:space="preserve">  , _ValueCategoryKey = </v>
+        <v xml:space="preserve">  , _ValueCategoryKey = 82000000093</v>
       </c>
       <c r="B5" s="12"/>
       <c r="C5" s="26"/>
       <c r="D5" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="35" t="str">
+      <c r="E5" s="35">
         <f>IF(ISBLANK('01 Function Comparison'!$H$3),"",'01 Function Comparison'!$H$3)</f>
-        <v/>
+        <v>82000000093</v>
       </c>
       <c r="F5" s="35"/>
     </row>
     <row r="6" spans="1:6" s="24" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="41" t="str">
         <f>CONCATENATE(D6,"N'",F6,"'")</f>
-        <v>WHERE _Name = N''</v>
+        <v>WHERE _Name = N'99RP264.1073742112SUPPLFX'</v>
       </c>
       <c r="B6" s="23"/>
       <c r="C6" s="30"/>
@@ -7574,27 +7614,27 @@
       <c r="E6" s="36"/>
       <c r="F6" s="36" t="str">
         <f>IF('01 Function Comparison'!$L$3="NULL","",IF(ISBLANK('01 Function Comparison'!$L$3),"",'01 Function Comparison'!$L$3))</f>
-        <v/>
+        <v>99RP264.1073742112SUPPLFX</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="38" t="str">
         <f>CONCATENATE(B7,C7,D7,E7)</f>
-        <v xml:space="preserve">-- Function: Massafra -   | Bergamo - </v>
+        <v>-- Function: Massafra -  25: Initial Malt to Maize Amount | Bergamo - 02: Initial Malt to Maize Amount</v>
       </c>
       <c r="B7" s="21" t="s">
         <v>31</v>
       </c>
       <c r="C7" s="29" t="str">
         <f>IF('01 Function Comparison'!$K$4="NULL","",IF(ISBLANK('01 Function Comparison'!$K$4),"",'01 Function Comparison'!$K$4))</f>
-        <v/>
+        <v>25: Initial Malt to Maize Amount</v>
       </c>
       <c r="D7" s="25" t="s">
         <v>23</v>
       </c>
       <c r="E7" s="34" t="str">
         <f>IF(ISBLANK('01 Function Comparison'!$G$4),"",'01 Function Comparison'!$G$4)</f>
-        <v/>
+        <v>02: Initial Malt to Maize Amount</v>
       </c>
       <c r="F7" s="42"/>
     </row>
@@ -7621,16 +7661,16 @@
     <row r="10" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="40" t="str">
         <f>CONCATENATE(D10,E10)</f>
-        <v xml:space="preserve">  , _ValueCategoryKey = </v>
+        <v xml:space="preserve">  , _ValueCategoryKey = 82000000029</v>
       </c>
       <c r="B10" s="12"/>
       <c r="C10" s="26"/>
       <c r="D10" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="35" t="str">
+      <c r="E10" s="35">
         <f>IF(ISBLANK('01 Function Comparison'!$H$4),"",'01 Function Comparison'!$H$4)</f>
-        <v/>
+        <v>82000000029</v>
       </c>
       <c r="F10" s="35"/>
     </row>
@@ -7653,21 +7693,21 @@
     <row r="12" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="38" t="str">
         <f>CONCATENATE(B12,C12,D12,E12)</f>
-        <v xml:space="preserve">-- Function: Massafra -   | Bergamo - </v>
+        <v>-- Function: Massafra -  26: Milling Time | Bergamo - 16: Milling Time</v>
       </c>
       <c r="B12" s="21" t="s">
         <v>31</v>
       </c>
       <c r="C12" s="29" t="str">
         <f>IF('01 Function Comparison'!$K$5="NULL","",IF(ISBLANK('01 Function Comparison'!$K$5),"",'01 Function Comparison'!$K$5))</f>
-        <v/>
+        <v>26: Milling Time</v>
       </c>
       <c r="D12" s="25" t="s">
         <v>23</v>
       </c>
       <c r="E12" s="34" t="str">
         <f>IF(ISBLANK('01 Function Comparison'!$G$5),"",'01 Function Comparison'!$G$5)</f>
-        <v/>
+        <v>16: Milling Time</v>
       </c>
       <c r="F12" s="42"/>
     </row>
@@ -7694,16 +7734,16 @@
     <row r="15" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="40" t="str">
         <f t="shared" ref="A15" si="0">CONCATENATE(D15,E15)</f>
-        <v xml:space="preserve">  , _ValueCategoryKey = </v>
+        <v xml:space="preserve">  , _ValueCategoryKey = 82000000091</v>
       </c>
       <c r="B15" s="12"/>
       <c r="C15" s="26"/>
       <c r="D15" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="35" t="str">
+      <c r="E15" s="35">
         <f>IF(ISBLANK('01 Function Comparison'!$H$5),"",'01 Function Comparison'!$H$5)</f>
-        <v/>
+        <v>82000000091</v>
       </c>
       <c r="F15" s="35"/>
     </row>
@@ -12394,7 +12434,7 @@
   <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:P8"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13549,8 +13589,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:P404"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13669,14 +13709,8 @@
       <c r="I3" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="2">
-        <v>7</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>33</v>
+      <c r="K3" s="57" t="s">
+        <v>36</v>
       </c>
       <c r="N3" s="11">
         <f>'00 Value Source'!H1</f>
@@ -13720,14 +13754,8 @@
       <c r="I4" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="J4" s="2">
-        <v>8</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>39</v>
+      <c r="K4" s="57" t="s">
+        <v>42</v>
       </c>
       <c r="N4" s="11">
         <f>'00 Value Source'!H2</f>
@@ -13772,13 +13800,13 @@
         <v>50</v>
       </c>
       <c r="J5" s="2">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>47</v>
+        <v>173</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>45</v>
+        <v>171</v>
       </c>
       <c r="N5" s="11">
         <f>'00 Value Source'!H3</f>
@@ -13823,13 +13851,13 @@
         <v>55</v>
       </c>
       <c r="J6" s="2">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>5</v>
+        <v>179</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>51</v>
+        <v>177</v>
       </c>
       <c r="N6" s="11">
         <f>'00 Value Source'!H4</f>
@@ -13873,14 +13901,14 @@
       <c r="I7" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="J7" s="2" t="s">
-        <v>3</v>
+      <c r="J7" s="2">
+        <v>6</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>3</v>
+        <v>185</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>3</v>
+        <v>183</v>
       </c>
       <c r="N7" s="11" t="str">
         <f>'00 Value Source'!H5</f>
@@ -13924,14 +13952,14 @@
       <c r="I8" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="J8" s="2" t="s">
-        <v>3</v>
+      <c r="J8" s="2">
+        <v>8</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="N8" s="11" t="str">
         <f>'00 Value Source'!H6</f>
@@ -13975,14 +14003,11 @@
       <c r="I9" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="J9" s="2">
-        <v>18</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="L9" s="4" t="s">
-        <v>62</v>
+      <c r="J9" s="59">
+        <v>68</v>
+      </c>
+      <c r="K9" s="57" t="s">
+        <v>65</v>
       </c>
       <c r="N9" s="11">
         <f>'00 Value Source'!H7</f>
@@ -14026,14 +14051,11 @@
       <c r="I10" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="J10" s="2">
-        <v>20</v>
-      </c>
-      <c r="K10" s="3" t="s">
+      <c r="J10" s="59">
         <v>70</v>
       </c>
-      <c r="L10" s="4" t="s">
-        <v>68</v>
+      <c r="K10" s="56" t="s">
+        <v>71</v>
       </c>
       <c r="N10" s="11">
         <f>'00 Value Source'!H8</f>
@@ -14077,14 +14099,11 @@
       <c r="I11" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="J11" s="2">
-        <v>23</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="L11" s="4" t="s">
-        <v>74</v>
+      <c r="J11" s="59">
+        <v>73</v>
+      </c>
+      <c r="K11" s="56" t="s">
+        <v>77</v>
       </c>
       <c r="N11" s="11">
         <f>'00 Value Source'!H9</f>
@@ -14128,11 +14147,11 @@
       <c r="I12" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="J12" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>3</v>
+      <c r="J12" s="59">
+        <v>75</v>
+      </c>
+      <c r="K12" s="57" t="s">
+        <v>270</v>
       </c>
       <c r="L12" s="4" t="s">
         <v>3</v>
@@ -14179,11 +14198,11 @@
       <c r="I13" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="J13" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>3</v>
+      <c r="J13" s="59">
+        <v>76</v>
+      </c>
+      <c r="K13" s="57" t="s">
+        <v>84</v>
       </c>
       <c r="L13" s="4" t="s">
         <v>3</v>
@@ -14230,11 +14249,11 @@
       <c r="I14" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="J14" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>3</v>
+      <c r="J14" s="59">
+        <v>77</v>
+      </c>
+      <c r="K14" s="57" t="s">
+        <v>271</v>
       </c>
       <c r="L14" s="4" t="s">
         <v>3</v>
@@ -14281,11 +14300,11 @@
       <c r="I15" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="J15" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K15" s="3" t="s">
-        <v>3</v>
+      <c r="J15" s="59">
+        <v>78</v>
+      </c>
+      <c r="K15" s="57" t="s">
+        <v>90</v>
       </c>
       <c r="L15" s="4" t="s">
         <v>3</v>
@@ -14332,11 +14351,11 @@
       <c r="I16" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="J16" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K16" s="3" t="s">
-        <v>3</v>
+      <c r="J16" s="59">
+        <v>79</v>
+      </c>
+      <c r="K16" s="57" t="s">
+        <v>272</v>
       </c>
       <c r="L16" s="4" t="s">
         <v>3</v>
@@ -14383,11 +14402,11 @@
       <c r="I17" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="J17" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K17" s="3" t="s">
-        <v>3</v>
+      <c r="J17" s="59">
+        <v>80</v>
+      </c>
+      <c r="K17" s="57" t="s">
+        <v>96</v>
       </c>
       <c r="L17" s="4" t="s">
         <v>3</v>
@@ -14434,11 +14453,11 @@
       <c r="I18" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="J18" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K18" s="3" t="s">
-        <v>3</v>
+      <c r="J18" s="59">
+        <v>81</v>
+      </c>
+      <c r="K18" s="57" t="s">
+        <v>273</v>
       </c>
       <c r="L18" s="4" t="s">
         <v>3</v>
@@ -14485,11 +14504,11 @@
       <c r="I19" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="J19" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K19" s="3" t="s">
-        <v>3</v>
+      <c r="J19" s="59">
+        <v>82</v>
+      </c>
+      <c r="K19" s="57" t="s">
+        <v>102</v>
       </c>
       <c r="L19" s="4" t="s">
         <v>3</v>
@@ -14539,8 +14558,8 @@
       <c r="J20" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K20" s="3" t="s">
-        <v>3</v>
+      <c r="K20" s="57" t="s">
+        <v>274</v>
       </c>
       <c r="L20" s="4" t="s">
         <v>3</v>
@@ -14590,8 +14609,8 @@
       <c r="J21" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K21" s="3" t="s">
-        <v>3</v>
+      <c r="K21" s="57" t="s">
+        <v>108</v>
       </c>
       <c r="L21" s="4" t="s">
         <v>3</v>
@@ -14641,8 +14660,8 @@
       <c r="J22" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K22" s="3" t="s">
-        <v>3</v>
+      <c r="K22" s="57" t="s">
+        <v>275</v>
       </c>
       <c r="L22" s="4" t="s">
         <v>3</v>
@@ -14692,8 +14711,8 @@
       <c r="J23" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K23" s="3" t="s">
-        <v>3</v>
+      <c r="K23" s="57" t="s">
+        <v>114</v>
       </c>
       <c r="L23" s="4" t="s">
         <v>3</v>
@@ -14743,8 +14762,8 @@
       <c r="J24" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K24" s="3" t="s">
-        <v>3</v>
+      <c r="K24" s="57" t="s">
+        <v>117</v>
       </c>
       <c r="L24" s="4" t="s">
         <v>3</v>
@@ -14794,8 +14813,8 @@
       <c r="J25" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K25" s="3" t="s">
-        <v>3</v>
+      <c r="K25" s="57" t="s">
+        <v>120</v>
       </c>
       <c r="L25" s="4" t="s">
         <v>3</v>
@@ -14845,8 +14864,8 @@
       <c r="J26" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K26" s="3" t="s">
-        <v>3</v>
+      <c r="K26" s="57" t="s">
+        <v>123</v>
       </c>
       <c r="L26" s="4" t="s">
         <v>3</v>
@@ -14896,8 +14915,8 @@
       <c r="J27" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K27" s="3" t="s">
-        <v>3</v>
+      <c r="K27" s="57" t="s">
+        <v>126</v>
       </c>
       <c r="L27" s="4" t="s">
         <v>3</v>
@@ -14947,8 +14966,8 @@
       <c r="J28" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K28" s="3" t="s">
-        <v>3</v>
+      <c r="K28" s="57" t="s">
+        <v>129</v>
       </c>
       <c r="L28" s="4" t="s">
         <v>3</v>
@@ -14998,8 +15017,8 @@
       <c r="J29" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K29" s="3" t="s">
-        <v>3</v>
+      <c r="K29" s="57" t="s">
+        <v>132</v>
       </c>
       <c r="L29" s="4" t="s">
         <v>3</v>
@@ -15049,8 +15068,8 @@
       <c r="J30" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K30" s="3" t="s">
-        <v>3</v>
+      <c r="K30" s="57" t="s">
+        <v>135</v>
       </c>
       <c r="L30" s="4" t="s">
         <v>3</v>
@@ -15100,8 +15119,8 @@
       <c r="J31" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K31" s="3" t="s">
-        <v>3</v>
+      <c r="K31" s="57" t="s">
+        <v>138</v>
       </c>
       <c r="L31" s="4" t="s">
         <v>3</v>
@@ -15151,8 +15170,8 @@
       <c r="J32" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K32" s="3" t="s">
-        <v>3</v>
+      <c r="K32" s="57" t="s">
+        <v>141</v>
       </c>
       <c r="L32" s="4" t="s">
         <v>3</v>
@@ -15202,8 +15221,8 @@
       <c r="J33" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K33" s="3" t="s">
-        <v>3</v>
+      <c r="K33" s="57" t="s">
+        <v>144</v>
       </c>
       <c r="L33" s="4" t="s">
         <v>3</v>
@@ -15253,8 +15272,8 @@
       <c r="J34" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K34" s="3" t="s">
-        <v>3</v>
+      <c r="K34" s="57" t="s">
+        <v>147</v>
       </c>
       <c r="L34" s="4" t="s">
         <v>3</v>
@@ -15304,8 +15323,8 @@
       <c r="J35" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K35" s="3" t="s">
-        <v>3</v>
+      <c r="K35" s="57" t="s">
+        <v>150</v>
       </c>
       <c r="L35" s="4" t="s">
         <v>3</v>
@@ -15355,8 +15374,8 @@
       <c r="J36" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K36" s="3" t="s">
-        <v>3</v>
+      <c r="K36" s="57" t="s">
+        <v>153</v>
       </c>
       <c r="L36" s="4" t="s">
         <v>3</v>
@@ -15406,8 +15425,8 @@
       <c r="J37" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K37" s="3" t="s">
-        <v>3</v>
+      <c r="K37" s="57" t="s">
+        <v>156</v>
       </c>
       <c r="L37" s="4" t="s">
         <v>3</v>
@@ -15457,8 +15476,8 @@
       <c r="J38" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K38" s="3" t="s">
-        <v>3</v>
+      <c r="K38" s="57" t="s">
+        <v>159</v>
       </c>
       <c r="L38" s="4" t="s">
         <v>3</v>
@@ -15508,8 +15527,8 @@
       <c r="J39" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K39" s="3" t="s">
-        <v>3</v>
+      <c r="K39" s="57" t="s">
+        <v>162</v>
       </c>
       <c r="L39" s="4" t="s">
         <v>3</v>
@@ -15559,8 +15578,8 @@
       <c r="J40" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K40" s="3" t="s">
-        <v>3</v>
+      <c r="K40" s="57" t="s">
+        <v>165</v>
       </c>
       <c r="L40" s="4" t="s">
         <v>3</v>
@@ -15595,15 +15614,6 @@
         <f>'00 Value Source'!P39</f>
         <v>NULL</v>
       </c>
-      <c r="J41" s="2">
-        <v>1</v>
-      </c>
-      <c r="K41" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="L41" s="4" t="s">
-        <v>168</v>
-      </c>
       <c r="N41" s="11">
         <f>'00 Value Source'!H39</f>
         <v>1</v>
@@ -15634,15 +15644,6 @@
         <f>'00 Value Source'!P40</f>
         <v>NULL</v>
       </c>
-      <c r="J42" s="2">
-        <v>2</v>
-      </c>
-      <c r="K42" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="L42" s="4" t="s">
-        <v>171</v>
-      </c>
       <c r="N42" s="11">
         <f>'00 Value Source'!H40</f>
         <v>2</v>
@@ -15673,15 +15674,6 @@
         <f>'00 Value Source'!P41</f>
         <v>NULL</v>
       </c>
-      <c r="J43" s="2">
-        <v>3</v>
-      </c>
-      <c r="K43" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="L43" s="4" t="s">
-        <v>174</v>
-      </c>
       <c r="N43" s="11">
         <f>'00 Value Source'!H41</f>
         <v>3</v>
@@ -15712,15 +15704,6 @@
         <f>'00 Value Source'!P42</f>
         <v>NULL</v>
       </c>
-      <c r="J44" s="2">
-        <v>4</v>
-      </c>
-      <c r="K44" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="L44" s="4" t="s">
-        <v>177</v>
-      </c>
       <c r="N44" s="11">
         <f>'00 Value Source'!H42</f>
         <v>4</v>
@@ -15751,15 +15734,6 @@
         <f>'00 Value Source'!P43</f>
         <v>NULL</v>
       </c>
-      <c r="J45" s="2">
-        <v>5</v>
-      </c>
-      <c r="K45" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="L45" s="4" t="s">
-        <v>180</v>
-      </c>
       <c r="N45" s="11">
         <f>'00 Value Source'!H43</f>
         <v>5</v>
@@ -15790,15 +15764,6 @@
         <f>'00 Value Source'!P44</f>
         <v>NULL</v>
       </c>
-      <c r="J46" s="2">
-        <v>6</v>
-      </c>
-      <c r="K46" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="L46" s="4" t="s">
-        <v>183</v>
-      </c>
       <c r="N46" s="11">
         <f>'00 Value Source'!H44</f>
         <v>6</v>
@@ -15829,15 +15794,6 @@
         <f>'00 Value Source'!P45</f>
         <v>NULL</v>
       </c>
-      <c r="J47" s="2">
-        <v>9</v>
-      </c>
-      <c r="K47" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="L47" s="4" t="s">
-        <v>186</v>
-      </c>
       <c r="N47" s="11">
         <f>'00 Value Source'!H45</f>
         <v>9</v>
@@ -15868,15 +15824,6 @@
         <f>'00 Value Source'!P46</f>
         <v>NULL</v>
       </c>
-      <c r="J48" s="2">
-        <v>11</v>
-      </c>
-      <c r="K48" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="L48" s="4" t="s">
-        <v>189</v>
-      </c>
       <c r="N48" s="11">
         <f>'00 Value Source'!H46</f>
         <v>11</v>
@@ -15907,15 +15854,6 @@
         <f>'00 Value Source'!P47</f>
         <v>NULL</v>
       </c>
-      <c r="J49" s="2">
-        <v>13</v>
-      </c>
-      <c r="K49" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="L49" s="4" t="s">
-        <v>192</v>
-      </c>
       <c r="N49" s="11">
         <f>'00 Value Source'!H47</f>
         <v>13</v>
@@ -15946,15 +15884,6 @@
         <f>'00 Value Source'!P48</f>
         <v>NULL</v>
       </c>
-      <c r="J50" s="2">
-        <v>19</v>
-      </c>
-      <c r="K50" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="L50" s="4" t="s">
-        <v>195</v>
-      </c>
       <c r="N50" s="11">
         <f>'00 Value Source'!H48</f>
         <v>19</v>
@@ -15984,15 +15913,6 @@
       <c r="D51" s="13" t="str">
         <f>'00 Value Source'!P49</f>
         <v>NULL</v>
-      </c>
-      <c r="J51" s="2">
-        <v>21</v>
-      </c>
-      <c r="K51" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="L51" s="4" t="s">
-        <v>198</v>
       </c>
       <c r="N51" s="11">
         <f>'00 Value Source'!H49</f>
@@ -20269,6 +20189,7 @@
     <mergeCell ref="N1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -26601,8 +26522,8 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:P404"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView topLeftCell="D1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -26709,6 +26630,27 @@
         <f>'00 Function Source'!P1</f>
         <v>Time Total Occupation - Extraction</v>
       </c>
+      <c r="F3" s="2">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="3">
+        <v>82000000093</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="J3" s="2">
+        <v>1</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>222</v>
+      </c>
       <c r="N3" s="11">
         <f>'00 Function Source'!H1</f>
         <v>1</v>
@@ -26739,6 +26681,21 @@
         <f>'00 Function Source'!P2</f>
         <v>Q.tà malto su cassone mais</v>
       </c>
+      <c r="F4" s="2">
+        <v>2</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="H4" s="3">
+        <v>82000000029</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="K4" s="58" t="s">
+        <v>269</v>
+      </c>
       <c r="N4" s="11" t="str">
         <f>'00 Function Source'!H2</f>
         <v>NULL</v>
@@ -26768,6 +26725,21 @@
       <c r="D5" s="13" t="str">
         <f>'00 Function Source'!P3</f>
         <v>Time Milling</v>
+      </c>
+      <c r="F5" s="2">
+        <v>16</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="H5" s="3">
+        <v>82000000091</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="K5" s="58" t="s">
+        <v>268</v>
       </c>
       <c r="N5" s="11">
         <f>'00 Function Source'!H3</f>
@@ -33320,8 +33292,8 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:T263"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -38475,14 +38447,14 @@
     <row r="2" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="38" t="str">
         <f>CONCATENATE(B2,C2,D2,E2)</f>
-        <v>-- Value: Massafra -  Malt amount Outtake 3 | Bergamo - 007: Special Malt Amaunt Outtake 1</v>
+        <v>-- Value: Massafra -  007: Special Malt Amaunt Outtake 1 | Bergamo - 007: Special Malt Amaunt Outtake 1</v>
       </c>
       <c r="B2" s="21" t="s">
         <v>24</v>
       </c>
       <c r="C2" s="29" t="str">
         <f>IF('01 Value Comparison'!$K$3="NULL","",IF(ISBLANK('01 Value Comparison'!$K$3),"",'01 Value Comparison'!$K$3))</f>
-        <v>Malt amount Outtake 3</v>
+        <v>007: Special Malt Amaunt Outtake 1</v>
       </c>
       <c r="D2" s="25" t="s">
         <v>23</v>
@@ -38532,7 +38504,7 @@
     <row r="6" spans="1:6" s="24" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="41" t="str">
         <f>CONCATENATE(D6,"N'",F6,"'")</f>
-        <v>WHERE _Name = N'99RP264.536871440SUPPLVA'</v>
+        <v>WHERE _Name = N''</v>
       </c>
       <c r="B6" s="23"/>
       <c r="C6" s="30"/>
@@ -38542,20 +38514,20 @@
       <c r="E6" s="36"/>
       <c r="F6" s="36" t="str">
         <f>IF('01 Value Comparison'!$L$3="NULL","",IF(ISBLANK('01 Value Comparison'!$L$3),"",'01 Value Comparison'!$L$3))</f>
-        <v>99RP264.536871440SUPPLVA</v>
+        <v/>
       </c>
     </row>
     <row r="7" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="38" t="str">
         <f>CONCATENATE(B7,C7,D7,E7)</f>
-        <v>-- Value: Massafra -  Malt type Outtake 4 | Bergamo - 008: Colorato Malt Amaunt Outtake 2</v>
+        <v>-- Value: Massafra -  008: Colorato Malt Amaunt Outtake 2 | Bergamo - 008: Colorato Malt Amaunt Outtake 2</v>
       </c>
       <c r="B7" s="21" t="s">
         <v>24</v>
       </c>
       <c r="C7" s="29" t="str">
         <f>IF('01 Value Comparison'!$K$4="NULL","",IF(ISBLANK('01 Value Comparison'!$K$4),"",'01 Value Comparison'!$K$4))</f>
-        <v>Malt type Outtake 4</v>
+        <v>008: Colorato Malt Amaunt Outtake 2</v>
       </c>
       <c r="D7" s="25" t="s">
         <v>23</v>
@@ -38605,7 +38577,7 @@
     <row r="11" spans="1:6" s="24" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="41" t="str">
         <f>CONCATENATE(D11,"N'",F11,"'")</f>
-        <v>WHERE _Name = N'99RP264.536871441SUPPLVA'</v>
+        <v>WHERE _Name = N''</v>
       </c>
       <c r="B11" s="23"/>
       <c r="C11" s="30"/>
@@ -38615,20 +38587,20 @@
       <c r="E11" s="36"/>
       <c r="F11" s="36" t="str">
         <f>IF('01 Value Comparison'!$L$4="NULL","",IF(ISBLANK('01 Value Comparison'!$L$4),"",'01 Value Comparison'!$L$4))</f>
-        <v>99RP264.536871441SUPPLVA</v>
+        <v/>
       </c>
     </row>
     <row r="12" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="38" t="str">
         <f>CONCATENATE(B12,C12,D12,E12)</f>
-        <v>-- Value: Massafra -  Mill direction Counter | Bergamo - Malt Type Outtake 1</v>
+        <v>-- Value: Massafra -  Malt type Outtake 1 | Bergamo - Malt Type Outtake 1</v>
       </c>
       <c r="B12" s="21" t="s">
         <v>24</v>
       </c>
       <c r="C12" s="29" t="str">
         <f>IF('01 Value Comparison'!$K$5="NULL","",IF(ISBLANK('01 Value Comparison'!$K$5),"",'01 Value Comparison'!$K$5))</f>
-        <v>Mill direction Counter</v>
+        <v>Malt type Outtake 1</v>
       </c>
       <c r="D12" s="25" t="s">
         <v>23</v>
@@ -38678,7 +38650,7 @@
     <row r="16" spans="1:6" s="24" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="41" t="str">
         <f>CONCATENATE(D16,"N'",F16,"'")</f>
-        <v>WHERE _Name = N'99RP264.536871527SUPPLVA'</v>
+        <v>WHERE _Name = N'99RP264.536871435SUPPLVA'</v>
       </c>
       <c r="B16" s="23"/>
       <c r="C16" s="30"/>
@@ -38688,20 +38660,20 @@
       <c r="E16" s="36"/>
       <c r="F16" s="36" t="str">
         <f>IF('01 Value Comparison'!$L$5="NULL","",IF(ISBLANK('01 Value Comparison'!$L$5),"",'01 Value Comparison'!$L$5))</f>
-        <v>99RP264.536871527SUPPLVA</v>
+        <v>99RP264.536871435SUPPLVA</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="38" t="str">
         <f>CONCATENATE(B17,C17,D17,E17)</f>
-        <v>-- Value: Massafra -  Raw material total | Bergamo - Malt Type Outtake 2</v>
+        <v>-- Value: Massafra -  Malt type Outtake 2 | Bergamo - Malt Type Outtake 2</v>
       </c>
       <c r="B17" s="21" t="s">
         <v>24</v>
       </c>
       <c r="C17" s="29" t="str">
         <f>IF('01 Value Comparison'!$K$6="NULL","",IF(ISBLANK('01 Value Comparison'!$K$6),"",'01 Value Comparison'!$K$6))</f>
-        <v>Raw material total</v>
+        <v>Malt type Outtake 2</v>
       </c>
       <c r="D17" s="25" t="s">
         <v>23</v>
@@ -38751,7 +38723,7 @@
     <row r="21" spans="1:6" s="24" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="41" t="str">
         <f>CONCATENATE(D21,"N'",F21,"'")</f>
-        <v>WHERE _Name = N'99RP264.536873738SUPPLVA'</v>
+        <v>WHERE _Name = N'99RP264.536871437SUPPLVA'</v>
       </c>
       <c r="B21" s="23"/>
       <c r="C21" s="30"/>
@@ -38761,20 +38733,20 @@
       <c r="E21" s="36"/>
       <c r="F21" s="36" t="str">
         <f>IF('01 Value Comparison'!$L$6="NULL","",IF(ISBLANK('01 Value Comparison'!$L$6),"",'01 Value Comparison'!$L$6))</f>
-        <v>99RP264.536873738SUPPLVA</v>
+        <v>99RP264.536871437SUPPLVA</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="38" t="str">
         <f>CONCATENATE(B22,C22,D22,E22)</f>
-        <v>-- Value: Massafra -   | Bergamo - Malt Type Outtake 3</v>
+        <v>-- Value: Massafra -  Malt type Outtake 3 | Bergamo - Malt Type Outtake 3</v>
       </c>
       <c r="B22" s="21" t="s">
         <v>24</v>
       </c>
       <c r="C22" s="29" t="str">
         <f>IF('01 Value Comparison'!$K$7="NULL","",IF(ISBLANK('01 Value Comparison'!$K$7),"",'01 Value Comparison'!$K$7))</f>
-        <v/>
+        <v>Malt type Outtake 3</v>
       </c>
       <c r="D22" s="25" t="s">
         <v>23</v>
@@ -38824,7 +38796,7 @@
     <row r="26" spans="1:6" s="24" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="41" t="str">
         <f>CONCATENATE(D26,"N'",F26,"'")</f>
-        <v>WHERE _Name = N''</v>
+        <v>WHERE _Name = N'99RP264.536871439SUPPLVA'</v>
       </c>
       <c r="B26" s="23"/>
       <c r="C26" s="30"/>
@@ -38834,20 +38806,20 @@
       <c r="E26" s="36"/>
       <c r="F26" s="36" t="str">
         <f>IF('01 Value Comparison'!$L$7="NULL","",IF(ISBLANK('01 Value Comparison'!$L$7),"",'01 Value Comparison'!$L$7))</f>
-        <v/>
+        <v>99RP264.536871439SUPPLVA</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="38" t="str">
         <f>CONCATENATE(B27,C27,D27,E27)</f>
-        <v>-- Value: Massafra -   | Bergamo - Malt Type Outtake 4</v>
+        <v>-- Value: Massafra -  Malt type Outtake 4 | Bergamo - Malt Type Outtake 4</v>
       </c>
       <c r="B27" s="21" t="s">
         <v>24</v>
       </c>
       <c r="C27" s="29" t="str">
         <f>IF('01 Value Comparison'!$K$8="NULL","",IF(ISBLANK('01 Value Comparison'!$K$8),"",'01 Value Comparison'!$K$8))</f>
-        <v/>
+        <v>Malt type Outtake 4</v>
       </c>
       <c r="D27" s="25" t="s">
         <v>23</v>
@@ -38897,7 +38869,7 @@
     <row r="31" spans="1:6" s="24" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="41" t="str">
         <f>CONCATENATE(D31,"N'",F31,"'")</f>
-        <v>WHERE _Name = N''</v>
+        <v>WHERE _Name = N'99RP264.536871441SUPPLVA'</v>
       </c>
       <c r="B31" s="23"/>
       <c r="C31" s="30"/>
@@ -38907,20 +38879,20 @@
       <c r="E31" s="36"/>
       <c r="F31" s="36" t="str">
         <f>IF('01 Value Comparison'!$L$8="NULL","",IF(ISBLANK('01 Value Comparison'!$L$8),"",'01 Value Comparison'!$L$8))</f>
-        <v/>
+        <v>99RP264.536871441SUPPLVA</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="38" t="str">
         <f>CONCATENATE(B32,C32,D32,E32)</f>
-        <v>-- Value: Massafra -  Malt amount scale Outtake 1 | Bergamo - 018: Special Malt Type Outtake 1</v>
+        <v>-- Value: Massafra -  018: Special Malt Type Outtake 1 | Bergamo - 018: Special Malt Type Outtake 1</v>
       </c>
       <c r="B32" s="21" t="s">
         <v>24</v>
       </c>
       <c r="C32" s="29" t="str">
         <f>IF('01 Value Comparison'!$K$9="NULL","",IF(ISBLANK('01 Value Comparison'!$K$9),"",'01 Value Comparison'!$K$9))</f>
-        <v>Malt amount scale Outtake 1</v>
+        <v>018: Special Malt Type Outtake 1</v>
       </c>
       <c r="D32" s="25" t="s">
         <v>23</v>
@@ -38970,7 +38942,7 @@
     <row r="36" spans="1:6" s="24" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="41" t="str">
         <f>CONCATENATE(D36,"N'",F36,"'")</f>
-        <v>WHERE _Name = N'99RP264.536873930SUPPLVA'</v>
+        <v>WHERE _Name = N''</v>
       </c>
       <c r="B36" s="23"/>
       <c r="C36" s="30"/>
@@ -38980,20 +38952,20 @@
       <c r="E36" s="36"/>
       <c r="F36" s="36" t="str">
         <f>IF('01 Value Comparison'!$L$9="NULL","",IF(ISBLANK('01 Value Comparison'!$L$9),"",'01 Value Comparison'!$L$9))</f>
-        <v>99RP264.536873930SUPPLVA</v>
+        <v/>
       </c>
     </row>
     <row r="37" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="38" t="str">
         <f>CONCATENATE(B37,C37,D37,E37)</f>
-        <v>-- Value: Massafra -  Malt amount scale Outtake 3 | Bergamo - 020: Colorato Malt Type Outtake 1</v>
+        <v>-- Value: Massafra -  020: Colorato Malt Type Outtake 1 | Bergamo - 020: Colorato Malt Type Outtake 1</v>
       </c>
       <c r="B37" s="21" t="s">
         <v>24</v>
       </c>
       <c r="C37" s="29" t="str">
         <f>IF('01 Value Comparison'!$K$10="NULL","",IF(ISBLANK('01 Value Comparison'!$K$10),"",'01 Value Comparison'!$K$10))</f>
-        <v>Malt amount scale Outtake 3</v>
+        <v>020: Colorato Malt Type Outtake 1</v>
       </c>
       <c r="D37" s="25" t="s">
         <v>23</v>
@@ -39043,7 +39015,7 @@
     <row r="41" spans="1:6" s="24" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="41" t="str">
         <f>CONCATENATE(D41,"N'",F41,"'")</f>
-        <v>WHERE _Name = N'99RP264.536873932SUPPLVA'</v>
+        <v>WHERE _Name = N''</v>
       </c>
       <c r="B41" s="23"/>
       <c r="C41" s="30"/>
@@ -39053,20 +39025,20 @@
       <c r="E41" s="36"/>
       <c r="F41" s="36" t="str">
         <f>IF('01 Value Comparison'!$L$10="NULL","",IF(ISBLANK('01 Value Comparison'!$L$10),"",'01 Value Comparison'!$L$10))</f>
-        <v>99RP264.536873932SUPPLVA</v>
+        <v/>
       </c>
     </row>
     <row r="42" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="38" t="str">
         <f>CONCATENATE(B42,C42,D42,E42)</f>
-        <v>-- Value: Massafra -  Limit low flow | Bergamo - 023: MES UTIF Malt</v>
+        <v>-- Value: Massafra -  023: MES UTIF Malt | Bergamo - 023: MES UTIF Malt</v>
       </c>
       <c r="B42" s="21" t="s">
         <v>24</v>
       </c>
       <c r="C42" s="29" t="str">
         <f>IF('01 Value Comparison'!$K$11="NULL","",IF(ISBLANK('01 Value Comparison'!$K$11),"",'01 Value Comparison'!$K$11))</f>
-        <v>Limit low flow</v>
+        <v>023: MES UTIF Malt</v>
       </c>
       <c r="D42" s="25" t="s">
         <v>23</v>
@@ -39116,7 +39088,7 @@
     <row r="46" spans="1:6" s="24" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="41" t="str">
         <f>CONCATENATE(D46,"N'",F46,"'")</f>
-        <v>WHERE _Name = N'99RP264.536873993SUPPLVA'</v>
+        <v>WHERE _Name = N''</v>
       </c>
       <c r="B46" s="23"/>
       <c r="C46" s="30"/>
@@ -39126,20 +39098,20 @@
       <c r="E46" s="36"/>
       <c r="F46" s="36" t="str">
         <f>IF('01 Value Comparison'!$L$11="NULL","",IF(ISBLANK('01 Value Comparison'!$L$11),"",'01 Value Comparison'!$L$11))</f>
-        <v>99RP264.536873993SUPPLVA</v>
+        <v/>
       </c>
     </row>
     <row r="47" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="38" t="str">
         <f>CONCATENATE(B47,C47,D47,E47)</f>
-        <v>-- Value: Massafra -   | Bergamo - Silo Nr  Outtake 1</v>
+        <v>-- Value: Massafra -  025: Silo Nr  Outtake 1 | Bergamo - Silo Nr  Outtake 1</v>
       </c>
       <c r="B47" s="21" t="s">
         <v>24</v>
       </c>
       <c r="C47" s="29" t="str">
         <f>IF('01 Value Comparison'!$K$12="NULL","",IF(ISBLANK('01 Value Comparison'!$K$12),"",'01 Value Comparison'!$K$12))</f>
-        <v/>
+        <v>025: Silo Nr  Outtake 1</v>
       </c>
       <c r="D47" s="25" t="s">
         <v>23</v>
@@ -39205,14 +39177,14 @@
     <row r="52" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="38" t="str">
         <f>CONCATENATE(B52,C52,D52,E52)</f>
-        <v>-- Value: Massafra -   | Bergamo - 026: Stanby Silo Nr  Outtake 1</v>
+        <v>-- Value: Massafra -  026: Stanby Silo Nr  Outtake 1 | Bergamo - 026: Stanby Silo Nr  Outtake 1</v>
       </c>
       <c r="B52" s="21" t="s">
         <v>24</v>
       </c>
       <c r="C52" s="29" t="str">
         <f>IF('01 Value Comparison'!$K$13="NULL","",IF(ISBLANK('01 Value Comparison'!$K$13),"",'01 Value Comparison'!$K$13))</f>
-        <v/>
+        <v>026: Stanby Silo Nr  Outtake 1</v>
       </c>
       <c r="D52" s="25" t="s">
         <v>23</v>
@@ -39278,14 +39250,14 @@
     <row r="57" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="38" t="str">
         <f>CONCATENATE(B57,C57,D57,E57)</f>
-        <v>-- Value: Massafra -   | Bergamo - Silo Nr Outtake 2</v>
+        <v>-- Value: Massafra -  027: Silo Nr Outtake 2 | Bergamo - Silo Nr Outtake 2</v>
       </c>
       <c r="B57" s="21" t="s">
         <v>24</v>
       </c>
       <c r="C57" s="29" t="str">
         <f>IF('01 Value Comparison'!$K$14="NULL","",IF(ISBLANK('01 Value Comparison'!$K$14),"",'01 Value Comparison'!$K$14))</f>
-        <v/>
+        <v>027: Silo Nr Outtake 2</v>
       </c>
       <c r="D57" s="25" t="s">
         <v>23</v>
@@ -39351,14 +39323,14 @@
     <row r="62" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="38" t="str">
         <f>CONCATENATE(B62,C62,D62,E62)</f>
-        <v>-- Value: Massafra -   | Bergamo - 028: Stanby Silo Nr Outtake 2</v>
+        <v>-- Value: Massafra -  028: Stanby Silo Nr Outtake 2 | Bergamo - 028: Stanby Silo Nr Outtake 2</v>
       </c>
       <c r="B62" s="21" t="s">
         <v>24</v>
       </c>
       <c r="C62" s="29" t="str">
         <f>IF('01 Value Comparison'!$K$15="NULL","",IF(ISBLANK('01 Value Comparison'!$K$15),"",'01 Value Comparison'!$K$15))</f>
-        <v/>
+        <v>028: Stanby Silo Nr Outtake 2</v>
       </c>
       <c r="D62" s="25" t="s">
         <v>23</v>
@@ -39424,14 +39396,14 @@
     <row r="67" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" s="38" t="str">
         <f>CONCATENATE(B67,C67,D67,E67)</f>
-        <v>-- Value: Massafra -   | Bergamo - Silo Nr Outtake 3</v>
+        <v>-- Value: Massafra -  029: Silo Nr Outtake 3 | Bergamo - Silo Nr Outtake 3</v>
       </c>
       <c r="B67" s="21" t="s">
         <v>24</v>
       </c>
       <c r="C67" s="29" t="str">
         <f>IF('01 Value Comparison'!$K$16="NULL","",IF(ISBLANK('01 Value Comparison'!$K$16),"",'01 Value Comparison'!$K$16))</f>
-        <v/>
+        <v>029: Silo Nr Outtake 3</v>
       </c>
       <c r="D67" s="25" t="s">
         <v>23</v>
@@ -39497,14 +39469,14 @@
     <row r="72" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A72" s="38" t="str">
         <f>CONCATENATE(B72,C72,D72,E72)</f>
-        <v>-- Value: Massafra -   | Bergamo - 030: Stanby Silo Nr Outtake 3</v>
+        <v>-- Value: Massafra -  030: Stanby Silo Nr Outtake 3 | Bergamo - 030: Stanby Silo Nr Outtake 3</v>
       </c>
       <c r="B72" s="21" t="s">
         <v>24</v>
       </c>
       <c r="C72" s="29" t="str">
         <f>IF('01 Value Comparison'!$K$17="NULL","",IF(ISBLANK('01 Value Comparison'!$K$17),"",'01 Value Comparison'!$K$17))</f>
-        <v/>
+        <v>030: Stanby Silo Nr Outtake 3</v>
       </c>
       <c r="D72" s="25" t="s">
         <v>23</v>
@@ -39570,14 +39542,14 @@
     <row r="77" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A77" s="38" t="str">
         <f>CONCATENATE(B77,C77,D77,E77)</f>
-        <v>-- Value: Massafra -   | Bergamo - Silo Nr Outtake 4</v>
+        <v>-- Value: Massafra -  031: Silo Nr Outtake 4 | Bergamo - Silo Nr Outtake 4</v>
       </c>
       <c r="B77" s="21" t="s">
         <v>24</v>
       </c>
       <c r="C77" s="29" t="str">
         <f>IF('01 Value Comparison'!$K$18="NULL","",IF(ISBLANK('01 Value Comparison'!$K$18),"",'01 Value Comparison'!$K$18))</f>
-        <v/>
+        <v>031: Silo Nr Outtake 4</v>
       </c>
       <c r="D77" s="25" t="s">
         <v>23</v>
@@ -39643,14 +39615,14 @@
     <row r="82" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A82" s="38" t="str">
         <f>CONCATENATE(B82,C82,D82,E82)</f>
-        <v>-- Value: Massafra -   | Bergamo - 032: Stanby Silo Nr Outtake 4</v>
+        <v>-- Value: Massafra -  032: Stanby Silo Nr Outtake 4 | Bergamo - 032: Stanby Silo Nr Outtake 4</v>
       </c>
       <c r="B82" s="21" t="s">
         <v>24</v>
       </c>
       <c r="C82" s="29" t="str">
         <f>IF('01 Value Comparison'!$K$19="NULL","",IF(ISBLANK('01 Value Comparison'!$K$19),"",'01 Value Comparison'!$K$19))</f>
-        <v/>
+        <v>032: Stanby Silo Nr Outtake 4</v>
       </c>
       <c r="D82" s="25" t="s">
         <v>23</v>
@@ -39716,14 +39688,14 @@
     <row r="87" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A87" s="38" t="str">
         <f>CONCATENATE(B87,C87,D87,E87)</f>
-        <v>-- Value: Massafra -   | Bergamo - Silo Nr Outtake Special</v>
+        <v>-- Value: Massafra -  033: Silo Nr Outtake Special | Bergamo - Silo Nr Outtake Special</v>
       </c>
       <c r="B87" s="21" t="s">
         <v>24</v>
       </c>
       <c r="C87" s="29" t="str">
         <f>IF('01 Value Comparison'!$K$20="NULL","",IF(ISBLANK('01 Value Comparison'!$K$20),"",'01 Value Comparison'!$K$20))</f>
-        <v/>
+        <v>033: Silo Nr Outtake Special</v>
       </c>
       <c r="D87" s="25" t="s">
         <v>23</v>
@@ -39789,14 +39761,14 @@
     <row r="92" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A92" s="38" t="str">
         <f>CONCATENATE(B92,C92,D92,E92)</f>
-        <v>-- Value: Massafra -   | Bergamo - 034: Stanby Silo Nr Outtake Special</v>
+        <v>-- Value: Massafra -  034: Stanby Silo Nr Outtake Special | Bergamo - 034: Stanby Silo Nr Outtake Special</v>
       </c>
       <c r="B92" s="21" t="s">
         <v>24</v>
       </c>
       <c r="C92" s="29" t="str">
         <f>IF('01 Value Comparison'!$K$21="NULL","",IF(ISBLANK('01 Value Comparison'!$K$21),"",'01 Value Comparison'!$K$21))</f>
-        <v/>
+        <v>034: Stanby Silo Nr Outtake Special</v>
       </c>
       <c r="D92" s="25" t="s">
         <v>23</v>
@@ -39862,14 +39834,14 @@
     <row r="97" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A97" s="38" t="str">
         <f>CONCATENATE(B97,C97,D97,E97)</f>
-        <v>-- Value: Massafra -   | Bergamo - Silo Nr Outtake Colorato</v>
+        <v>-- Value: Massafra -  035: Silo Nr Outtake Colorato | Bergamo - Silo Nr Outtake Colorato</v>
       </c>
       <c r="B97" s="21" t="s">
         <v>24</v>
       </c>
       <c r="C97" s="29" t="str">
         <f>IF('01 Value Comparison'!$K$22="NULL","",IF(ISBLANK('01 Value Comparison'!$K$22),"",'01 Value Comparison'!$K$22))</f>
-        <v/>
+        <v>035: Silo Nr Outtake Colorato</v>
       </c>
       <c r="D97" s="25" t="s">
         <v>23</v>
@@ -39935,14 +39907,14 @@
     <row r="102" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A102" s="38" t="str">
         <f>CONCATENATE(B102,C102,D102,E102)</f>
-        <v>-- Value: Massafra -   | Bergamo - 037: Yield Outtake 1</v>
+        <v>-- Value: Massafra -  037: Yield Outtake 1 | Bergamo - 037: Yield Outtake 1</v>
       </c>
       <c r="B102" s="21" t="s">
         <v>24</v>
       </c>
       <c r="C102" s="29" t="str">
         <f>IF('01 Value Comparison'!$K$23="NULL","",IF(ISBLANK('01 Value Comparison'!$K$23),"",'01 Value Comparison'!$K$23))</f>
-        <v/>
+        <v>037: Yield Outtake 1</v>
       </c>
       <c r="D102" s="25" t="s">
         <v>23</v>
@@ -40008,14 +39980,14 @@
     <row r="107" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A107" s="38" t="str">
         <f>CONCATENATE(B107,C107,D107,E107)</f>
-        <v>-- Value: Massafra -   | Bergamo - 038: Yield Outtake 2</v>
+        <v>-- Value: Massafra -  038: Yield Outtake 2 | Bergamo - 038: Yield Outtake 2</v>
       </c>
       <c r="B107" s="21" t="s">
         <v>24</v>
       </c>
       <c r="C107" s="29" t="str">
         <f>IF('01 Value Comparison'!$K$24="NULL","",IF(ISBLANK('01 Value Comparison'!$K$24),"",'01 Value Comparison'!$K$24))</f>
-        <v/>
+        <v>038: Yield Outtake 2</v>
       </c>
       <c r="D107" s="25" t="s">
         <v>23</v>
@@ -40081,14 +40053,14 @@
     <row r="112" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A112" s="38" t="str">
         <f>CONCATENATE(B112,C112,D112,E112)</f>
-        <v>-- Value: Massafra -   | Bergamo - 039: Yield Outtake 3</v>
+        <v>-- Value: Massafra -  039: Yield Outtake 3 | Bergamo - 039: Yield Outtake 3</v>
       </c>
       <c r="B112" s="21" t="s">
         <v>24</v>
       </c>
       <c r="C112" s="29" t="str">
         <f>IF('01 Value Comparison'!$K$25="NULL","",IF(ISBLANK('01 Value Comparison'!$K$25),"",'01 Value Comparison'!$K$25))</f>
-        <v/>
+        <v>039: Yield Outtake 3</v>
       </c>
       <c r="D112" s="25" t="s">
         <v>23</v>
@@ -40154,14 +40126,14 @@
     <row r="117" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A117" s="38" t="str">
         <f>CONCATENATE(B117,C117,D117,E117)</f>
-        <v>-- Value: Massafra -   | Bergamo - 040: Yield Outtake 4</v>
+        <v>-- Value: Massafra -  040: Yield Outtake 4 | Bergamo - 040: Yield Outtake 4</v>
       </c>
       <c r="B117" s="21" t="s">
         <v>24</v>
       </c>
       <c r="C117" s="29" t="str">
         <f>IF('01 Value Comparison'!$K$26="NULL","",IF(ISBLANK('01 Value Comparison'!$K$26),"",'01 Value Comparison'!$K$26))</f>
-        <v/>
+        <v>040: Yield Outtake 4</v>
       </c>
       <c r="D117" s="25" t="s">
         <v>23</v>
@@ -40227,14 +40199,14 @@
     <row r="122" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A122" s="38" t="str">
         <f>CONCATENATE(B122,C122,D122,E122)</f>
-        <v>-- Value: Massafra -   | Bergamo - 042: Main Outtake 01</v>
+        <v>-- Value: Massafra -  042: Main Outtake 01 | Bergamo - 042: Main Outtake 01</v>
       </c>
       <c r="B122" s="21" t="s">
         <v>24</v>
       </c>
       <c r="C122" s="29" t="str">
         <f>IF('01 Value Comparison'!$K$27="NULL","",IF(ISBLANK('01 Value Comparison'!$K$27),"",'01 Value Comparison'!$K$27))</f>
-        <v/>
+        <v>042: Main Outtake 01</v>
       </c>
       <c r="D122" s="25" t="s">
         <v>23</v>
@@ -40300,14 +40272,14 @@
     <row r="127" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A127" s="38" t="str">
         <f>CONCATENATE(B127,C127,D127,E127)</f>
-        <v>-- Value: Massafra -   | Bergamo - 043: Main Outtake 02</v>
+        <v>-- Value: Massafra -  043: Main Outtake 02 | Bergamo - 043: Main Outtake 02</v>
       </c>
       <c r="B127" s="21" t="s">
         <v>24</v>
       </c>
       <c r="C127" s="29" t="str">
         <f>IF('01 Value Comparison'!$K$28="NULL","",IF(ISBLANK('01 Value Comparison'!$K$28),"",'01 Value Comparison'!$K$28))</f>
-        <v/>
+        <v>043: Main Outtake 02</v>
       </c>
       <c r="D127" s="25" t="s">
         <v>23</v>
@@ -40373,14 +40345,14 @@
     <row r="132" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A132" s="38" t="str">
         <f>CONCATENATE(B132,C132,D132,E132)</f>
-        <v>-- Value: Massafra -   | Bergamo - 044: Main Outtake 03</v>
+        <v>-- Value: Massafra -  044: Main Outtake 03 | Bergamo - 044: Main Outtake 03</v>
       </c>
       <c r="B132" s="21" t="s">
         <v>24</v>
       </c>
       <c r="C132" s="29" t="str">
         <f>IF('01 Value Comparison'!$K$29="NULL","",IF(ISBLANK('01 Value Comparison'!$K$29),"",'01 Value Comparison'!$K$29))</f>
-        <v/>
+        <v>044: Main Outtake 03</v>
       </c>
       <c r="D132" s="25" t="s">
         <v>23</v>
@@ -40446,14 +40418,14 @@
     <row r="137" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A137" s="38" t="str">
         <f>CONCATENATE(B137,C137,D137,E137)</f>
-        <v>-- Value: Massafra -   | Bergamo - 045: Main Outtake 04</v>
+        <v>-- Value: Massafra -  045: Main Outtake 04 | Bergamo - 045: Main Outtake 04</v>
       </c>
       <c r="B137" s="21" t="s">
         <v>24</v>
       </c>
       <c r="C137" s="29" t="str">
         <f>IF('01 Value Comparison'!$K$30="NULL","",IF(ISBLANK('01 Value Comparison'!$K$30),"",'01 Value Comparison'!$K$30))</f>
-        <v/>
+        <v>045: Main Outtake 04</v>
       </c>
       <c r="D137" s="25" t="s">
         <v>23</v>
@@ -40519,14 +40491,14 @@
     <row r="142" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A142" s="38" t="str">
         <f t="shared" ref="A142" si="4">CONCATENATE(B142,C142,D142,E142)</f>
-        <v>-- Value: Massafra -   | Bergamo - 046: Standby Outtake 01</v>
+        <v>-- Value: Massafra -  046: Standby Outtake 01 | Bergamo - 046: Standby Outtake 01</v>
       </c>
       <c r="B142" s="21" t="s">
         <v>24</v>
       </c>
       <c r="C142" s="29" t="str">
         <f>IF('01 Value Comparison'!$K$31="NULL","",IF(ISBLANK('01 Value Comparison'!$K$31),"",'01 Value Comparison'!$K$31))</f>
-        <v/>
+        <v>046: Standby Outtake 01</v>
       </c>
       <c r="D142" s="25" t="s">
         <v>23</v>
@@ -40592,14 +40564,14 @@
     <row r="147" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A147" s="38" t="str">
         <f t="shared" ref="A147" si="7">CONCATENATE(B147,C147,D147,E147)</f>
-        <v>-- Value: Massafra -   | Bergamo - 047: Standby Outtake 02</v>
+        <v>-- Value: Massafra -  047: Standby Outtake 02 | Bergamo - 047: Standby Outtake 02</v>
       </c>
       <c r="B147" s="21" t="s">
         <v>24</v>
       </c>
       <c r="C147" s="29" t="str">
         <f>IF('01 Value Comparison'!$K$32="NULL","",IF(ISBLANK('01 Value Comparison'!$K$32),"",'01 Value Comparison'!$K$32))</f>
-        <v/>
+        <v>047: Standby Outtake 02</v>
       </c>
       <c r="D147" s="25" t="s">
         <v>23</v>
@@ -40665,14 +40637,14 @@
     <row r="152" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A152" s="38" t="str">
         <f t="shared" ref="A152" si="10">CONCATENATE(B152,C152,D152,E152)</f>
-        <v>-- Value: Massafra -   | Bergamo - 048: Standby Outtake 03</v>
+        <v>-- Value: Massafra -  048: Standby Outtake 03 | Bergamo - 048: Standby Outtake 03</v>
       </c>
       <c r="B152" s="21" t="s">
         <v>24</v>
       </c>
       <c r="C152" s="29" t="str">
         <f>IF('01 Value Comparison'!$K$33="NULL","",IF(ISBLANK('01 Value Comparison'!$K$33),"",'01 Value Comparison'!$K$33))</f>
-        <v/>
+        <v>048: Standby Outtake 03</v>
       </c>
       <c r="D152" s="25" t="s">
         <v>23</v>
@@ -40738,14 +40710,14 @@
     <row r="157" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A157" s="38" t="str">
         <f t="shared" ref="A157" si="13">CONCATENATE(B157,C157,D157,E157)</f>
-        <v>-- Value: Massafra -   | Bergamo - 049: Standby Outtake 04</v>
+        <v>-- Value: Massafra -  049: Standby Outtake 04 | Bergamo - 049: Standby Outtake 04</v>
       </c>
       <c r="B157" s="21" t="s">
         <v>24</v>
       </c>
       <c r="C157" s="29" t="str">
         <f>IF('01 Value Comparison'!$K$34="NULL","",IF(ISBLANK('01 Value Comparison'!$K$34),"",'01 Value Comparison'!$K$34))</f>
-        <v/>
+        <v>049: Standby Outtake 04</v>
       </c>
       <c r="D157" s="25" t="s">
         <v>23</v>
@@ -40811,14 +40783,14 @@
     <row r="162" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A162" s="38" t="str">
         <f t="shared" ref="A162" si="16">CONCATENATE(B162,C162,D162,E162)</f>
-        <v>-- Value: Massafra -   | Bergamo - 058: Yield Standby Outtake 1</v>
+        <v>-- Value: Massafra -  058: Yield Standby Outtake 1 | Bergamo - 058: Yield Standby Outtake 1</v>
       </c>
       <c r="B162" s="21" t="s">
         <v>24</v>
       </c>
       <c r="C162" s="29" t="str">
         <f>IF('01 Value Comparison'!$K$35="NULL","",IF(ISBLANK('01 Value Comparison'!$K$35),"",'01 Value Comparison'!$K$35))</f>
-        <v/>
+        <v>058: Yield Standby Outtake 1</v>
       </c>
       <c r="D162" s="25" t="s">
         <v>23</v>
@@ -40884,14 +40856,14 @@
     <row r="167" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A167" s="38" t="str">
         <f t="shared" ref="A167" si="19">CONCATENATE(B167,C167,D167,E167)</f>
-        <v>-- Value: Massafra -   | Bergamo - 059: Yield Standby Outtake 2</v>
+        <v>-- Value: Massafra -  059: Yield Standby Outtake 2 | Bergamo - 059: Yield Standby Outtake 2</v>
       </c>
       <c r="B167" s="21" t="s">
         <v>24</v>
       </c>
       <c r="C167" s="29" t="str">
         <f>IF('01 Value Comparison'!$K$36="NULL","",IF(ISBLANK('01 Value Comparison'!$K$36),"",'01 Value Comparison'!$K$36))</f>
-        <v/>
+        <v>059: Yield Standby Outtake 2</v>
       </c>
       <c r="D167" s="25" t="s">
         <v>23</v>
@@ -40957,14 +40929,14 @@
     <row r="172" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A172" s="38" t="str">
         <f t="shared" ref="A172" si="22">CONCATENATE(B172,C172,D172,E172)</f>
-        <v>-- Value: Massafra -   | Bergamo - 060: Yield Standby Outtake 3</v>
+        <v>-- Value: Massafra -  0 | Bergamo - 060: Yield Standby Outtake 3</v>
       </c>
       <c r="B172" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C172" s="29" t="str">
+      <c r="C172" s="29">
         <f>IF('01 Value Comparison'!$K$37="NULL","",IF(ISBLANK('01 Value Comparison'!$K$37),"",'01 Value Comparison'!$K$47))</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="D172" s="25" t="s">
         <v>23</v>
@@ -41030,14 +41002,14 @@
     <row r="177" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A177" s="38" t="str">
         <f t="shared" ref="A177" si="25">CONCATENATE(B177,C177,D177,E177)</f>
-        <v>-- Value: Massafra -   | Bergamo - 061: Yield Standby Outtake 4</v>
+        <v>-- Value: Massafra -  061: Yield Standby Outtake 4 | Bergamo - 061: Yield Standby Outtake 4</v>
       </c>
       <c r="B177" s="21" t="s">
         <v>24</v>
       </c>
       <c r="C177" s="29" t="str">
         <f>IF('01 Value Comparison'!$K$38="NULL","",IF(ISBLANK('01 Value Comparison'!$K$38),"",'01 Value Comparison'!$K$38))</f>
-        <v/>
+        <v>061: Yield Standby Outtake 4</v>
       </c>
       <c r="D177" s="25" t="s">
         <v>23</v>
@@ -41103,14 +41075,14 @@
     <row r="182" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A182" s="38" t="str">
         <f t="shared" ref="A182" si="28">CONCATENATE(B182,C182,D182,E182)</f>
-        <v>-- Value: Massafra -   | Bergamo - 062: Coloured Yield</v>
+        <v>-- Value: Massafra -  062: Coloured Yield | Bergamo - 062: Coloured Yield</v>
       </c>
       <c r="B182" s="21" t="s">
         <v>24</v>
       </c>
       <c r="C182" s="29" t="str">
         <f>IF('01 Value Comparison'!$K$39="NULL","",IF(ISBLANK('01 Value Comparison'!$K$39),"",'01 Value Comparison'!$K$39))</f>
-        <v/>
+        <v>062: Coloured Yield</v>
       </c>
       <c r="D182" s="25" t="s">
         <v>23</v>
@@ -41176,14 +41148,14 @@
     <row r="187" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A187" s="38" t="str">
         <f t="shared" ref="A187" si="31">CONCATENATE(B187,C187,D187,E187)</f>
-        <v>-- Value: Massafra -   | Bergamo - 063: Special Yield</v>
+        <v>-- Value: Massafra -  063: Special Yield | Bergamo - 063: Special Yield</v>
       </c>
       <c r="B187" s="21" t="s">
         <v>24</v>
       </c>
       <c r="C187" s="29" t="str">
         <f>IF('01 Value Comparison'!$K$40="NULL","",IF(ISBLANK('01 Value Comparison'!$K$40),"",'01 Value Comparison'!$K$40))</f>
-        <v/>
+        <v>063: Special Yield</v>
       </c>
       <c r="D187" s="25" t="s">
         <v>23</v>

</xml_diff>